<commit_message>
updating CategoriaContratoFromTo test spreadsheet
</commit_message>
<xml_diff>
--- a/contratos/tests/data/test_CategoriaContratoFromToSpreadsheet.xlsx
+++ b/contratos/tests/data/test_CategoriaContratoFromToSpreadsheet.xlsx
@@ -14,6 +14,8 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tipologia!$A$1:$C$341</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Tipologia!$A$1:$C$341</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Tipologia!$A$1:$C$341</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Tipologia!$A$1:$C$341</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Tipologia!$A$1:$C$341</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +29,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
-    <t xml:space="preserve">indexador_dotacao_subelemento</t>
+    <t xml:space="preserve">indexador_dotacao</t>
   </si>
   <si>
     <t xml:space="preserve">Tipologia_CategContrato v3</t>
@@ -36,22 +38,22 @@
     <t xml:space="preserve">Texto explicativo (v1)</t>
   </si>
   <si>
-    <t xml:space="preserve">2018.16.2100.3.3.90.30.00.1</t>
+    <t xml:space="preserve">2018.16.2100.3.3.90.30.00</t>
   </si>
   <si>
-    <t xml:space="preserve">categoria</t>
+    <t xml:space="preserve">categoria </t>
   </si>
   <si>
-    <t xml:space="preserve">categoria desc</t>
+    <t xml:space="preserve">categoria desc </t>
   </si>
   <si>
-    <t xml:space="preserve">2018.16.2100.3.3.90.30.00.14</t>
+    <t xml:space="preserve">2018.16.2100.3.3.90.30.99</t>
   </si>
   <si>
-    <t xml:space="preserve">outra categoria</t>
+    <t xml:space="preserve">outra categoria </t>
   </si>
   <si>
-    <t xml:space="preserve">outra categoria desc</t>
+    <t xml:space="preserve">outra categoria desc </t>
   </si>
 </sst>
 </file>
@@ -185,7 +187,7 @@
   <dimension ref="A1:C65536"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>